<commit_message>
1.updated references 2.recent recrtment code
</commit_message>
<xml_diff>
--- a/recruitment/src/main/resources/Sanity.xlsx
+++ b/recruitment/src/main/resources/Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mouni\IdeaProjects\Master\Automation_Project\recruitment\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E0D9F1-9F9B-4E8B-96D3-0C18E695020B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBD5398-3737-4986-B1D1-BEE6580C8310}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
   <si>
     <t>TCID</t>
   </si>
@@ -123,6 +123,18 @@
   </si>
   <si>
     <t>com.darwinbox.recruitment.requisitions.TestJobPosting</t>
+  </si>
+  <si>
+    <t>JobPosting</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>com.darwinbox.recruitment.requisitions.TestHiringWorkFlow</t>
   </si>
 </sst>
 </file>
@@ -496,7 +508,7 @@
   <dimension ref="A1:H261"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -661,15 +673,37 @@
         <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>

</xml_diff>